<commit_message>
Suport relabeled pivot items
</commit_message>
<xml_diff>
--- a/tests/pivot_test.xlsx
+++ b/tests/pivot_test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/code/calamine/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CAE8E5-535C-BC46-84D0-BF3A7D260862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647C657C-1615-5443-9712-7BB610AFC802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7400" yWindow="3440" windowWidth="38000" windowHeight="21080" xr2:uid="{19EAE515-D135-7149-9A95-57D74D5B9153}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId3"/>
+    <pivotCache cacheId="6" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Product</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Average of Price</t>
+  </si>
+  <si>
+    <t>Renamed Orange</t>
   </si>
 </sst>
 </file>
@@ -108,14 +111,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -194,14 +196,14 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0D60B582-DDC9-8142-AD24-57A2D29E8B41}" name="SalesSummary" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0D60B582-DDC9-8142-AD24-57A2D29E8B41}" name="SalesSummary" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
         <item x="0"/>
-        <item x="1"/>
+        <item n="Renamed Orange" x="1"/>
         <item x="2"/>
         <item t="default"/>
       </items>
@@ -573,7 +575,7 @@
   <dimension ref="A3:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -598,21 +600,21 @@
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>0.55000000000000004</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4">
+        <v>11</v>
+      </c>
+      <c r="B5">
         <v>50</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5">
         <v>30</v>
       </c>
     </row>
@@ -620,10 +622,10 @@
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>0.3</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6">
         <v>20</v>
       </c>
     </row>
@@ -631,10 +633,10 @@
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>12.85</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <v>65</v>
       </c>
     </row>

</xml_diff>